<commit_message>
Alteração de algumas informações
</commit_message>
<xml_diff>
--- a/Documentações/Documentação inicial.xlsx
+++ b/Documentações/Documentação inicial.xlsx
@@ -10,8 +10,35 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="D4">
+      <text>
+        <t xml:space="preserve">*Qual o objetivo principal deste programa? 
+*Quais os objetivos secundários?
+*O que você espera otimizar
+ com este programa?</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="A7">
+      <text>
+        <t xml:space="preserve">*Nome fantasia
+*CNPJ
+*Telefones/e-mail
+*Representante
+*Descrição de produto</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Docsmanager</t>
   </si>
@@ -25,7 +52,7 @@
     <t>Solicitações do cliente</t>
   </si>
   <si>
-    <t>Tecnologias a serem utilizadas</t>
+    <t>Tecnologias a serem utilizadas e estudadas</t>
   </si>
   <si>
     <t>Armazenar comprovantes  e boletos pagos</t>
@@ -52,12 +79,18 @@
     <t>Apresentação do lucro e controle financeiro</t>
   </si>
   <si>
-    <t>Para interface gráfica (???)</t>
+    <t>Para interface gráfica (Java?Qt?Gtk?)</t>
   </si>
   <si>
     <t>Ter um campo de pesquisas de empresas cadastradas</t>
   </si>
   <si>
+    <t>Cadastrar os valores de fechamento do caixa</t>
+  </si>
+  <si>
+    <t>GitHub</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Identificar boletos pago (compensado ou não)</t>
   </si>
   <si>
@@ -70,10 +103,19 @@
     <t>Histórias</t>
   </si>
   <si>
+    <t>Responsáveis</t>
+  </si>
+  <si>
     <t>Relacionar o banco de dados</t>
   </si>
   <si>
+    <t>Victor França (Higlik) Java|Sql</t>
+  </si>
+  <si>
     <t>Criar um banco de dados para o armazenamento</t>
+  </si>
+  <si>
+    <t>João Victor (Vulgo Casas Bahia) Front|Interface</t>
   </si>
 </sst>
 </file>
@@ -104,7 +146,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,8 +167,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB7B7B7"/>
-        <bgColor rgb="FFB7B7B7"/>
+        <fgColor rgb="FFEFEFEF"/>
+        <bgColor rgb="FFEFEFEF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -208,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -228,12 +276,11 @@
     <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="4" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="8" fillId="4" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="4" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="5" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
     <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -495,7 +542,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I4" s="2"/>
@@ -573,17 +620,21 @@
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="9"/>
-      <c r="D9" s="12"/>
+      <c r="D9" s="11" t="s">
+        <v>15</v>
+      </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="9"/>
-      <c r="H9" s="12"/>
+      <c r="H9" s="11" t="s">
+        <v>16</v>
+      </c>
       <c r="I9" s="8"/>
       <c r="J9" s="9"/>
     </row>
     <row r="10">
       <c r="A10" s="11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="9"/>
@@ -597,7 +648,7 @@
     </row>
     <row r="11">
       <c r="A11" s="11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="9"/>
@@ -611,7 +662,7 @@
     </row>
     <row r="12">
       <c r="A12" s="11" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9"/>
@@ -625,7 +676,7 @@
     </row>
     <row r="13">
       <c r="A13" s="10" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="3"/>
@@ -633,9 +684,11 @@
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="9"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="9"/>
+      <c r="H13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="3"/>
     </row>
     <row r="14">
       <c r="A14" s="4"/>
@@ -645,13 +698,13 @@
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="9"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="9"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="6"/>
     </row>
     <row r="15">
       <c r="A15" s="11" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="9"/>
@@ -659,13 +712,15 @@
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="9"/>
-      <c r="H15" s="12"/>
+      <c r="H15" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="I15" s="8"/>
       <c r="J15" s="9"/>
     </row>
     <row r="16">
       <c r="A16" s="11" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="9"/>
@@ -673,30 +728,50 @@
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="9"/>
-      <c r="H16" s="12"/>
+      <c r="H16" s="11" t="s">
+        <v>25</v>
+      </c>
       <c r="I16" s="8"/>
       <c r="J16" s="9"/>
     </row>
     <row r="17">
       <c r="A17" s="13"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="15"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="39">
+    <mergeCell ref="A4:C5"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="H13:J14"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="A20:C20"/>
     <mergeCell ref="C1:H2"/>
     <mergeCell ref="C3:H3"/>
-    <mergeCell ref="A4:C5"/>
     <mergeCell ref="D4:G5"/>
     <mergeCell ref="H4:J5"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="A17:J17"/>
+    <mergeCell ref="D11:G11"/>
     <mergeCell ref="D6:G6"/>
     <mergeCell ref="H6:J6"/>
     <mergeCell ref="A6:C6"/>
@@ -705,34 +780,16 @@
     <mergeCell ref="H7:J7"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="D8:G8"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A19:C19"/>
     <mergeCell ref="A13:C14"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="D14:G14"/>
     <mergeCell ref="D15:G15"/>
     <mergeCell ref="D16:G16"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="H14:J14"/>
     <mergeCell ref="H15:J15"/>
     <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="A11:C11"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>